<commit_message>
add some information for np
</commit_message>
<xml_diff>
--- a/result_type.xlsx
+++ b/result_type.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\70916\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\70916\Desktop\TASINFER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{521F9FF4-082B-41E9-B251-D36DE5E59E7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C319200D-5508-4AC1-B3F3-EF6651264708}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-4965" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>比赛项目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -73,6 +73,14 @@
   </si>
   <si>
     <t>mypy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.kaggle.com/c/2018-hse-ml-competion-02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.kaggle.com/hippskill/press-vowpal-wabbit-to-win</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -412,16 +420,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="14.75" customWidth="1"/>
+    <col min="1" max="1" width="21.875" customWidth="1"/>
+    <col min="2" max="2" width="22.125" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
     <col min="4" max="4" width="10.125" customWidth="1"/>
     <col min="5" max="6" width="9.5" customWidth="1"/>
@@ -505,6 +513,43 @@
       <c r="K3">
         <f>(H3+I3)/C3</f>
         <v>0.90243902439024393</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>25</v>
+      </c>
+      <c r="D4">
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>8</v>
+      </c>
+      <c r="G4">
+        <f>(D4+E4)/C4</f>
+        <v>0.68</v>
+      </c>
+      <c r="H4">
+        <v>18</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>7</v>
+      </c>
+      <c r="K4">
+        <f>(H4+I4)/C4</f>
+        <v>0.72</v>
       </c>
     </row>
   </sheetData>
@@ -515,6 +560,8 @@
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{735C9856-19EB-420B-8C58-658AE0D7FFF4}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{B833D130-05D4-46EF-81B0-D11730AFE9F5}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{7478E201-8461-43FE-AC04-02AC45EFF772}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{FB424078-83DC-4591-B86A-945FE1A48C0C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>